<commit_message>
Graph from results to gap %
</commit_message>
<xml_diff>
--- a/PowerPoint/benchmarks(version 1).xlsx
+++ b/PowerPoint/benchmarks(version 1).xlsx
@@ -95,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +152,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +185,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -429,7 +442,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -483,6 +496,7 @@
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -846,11 +860,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="119"/>
-        <c:axId val="770505376"/>
-        <c:axId val="770507152"/>
+        <c:axId val="1978920352"/>
+        <c:axId val="1978922400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="770505376"/>
+        <c:axId val="1978920352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +921,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="770507152"/>
+        <c:crossAx val="1978922400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -915,7 +929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="770507152"/>
+        <c:axId val="1978922400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="770505376"/>
+        <c:crossAx val="1978920352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1924,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2123,10 +2137,12 @@
         <f>100*(U4-$G4)/$G4</f>
         <v>0.22050625585175493</v>
       </c>
-      <c r="W4" s="22"/>
+      <c r="W4" s="33">
+        <v>157.08099999999999</v>
+      </c>
       <c r="X4" s="23">
         <f>100*(W4-$G4)/$G4</f>
-        <v>-100</v>
+        <v>3.0736903751131559E-2</v>
       </c>
       <c r="Y4" s="22"/>
       <c r="Z4" s="23">
@@ -2205,10 +2221,12 @@
         <f t="shared" ref="V5:V10" si="6">100*(U5-$G5)/$G5</f>
         <v>12.982809556763959</v>
       </c>
-      <c r="W5" s="21"/>
+      <c r="W5" s="33">
+        <v>37.462000000000003</v>
+      </c>
       <c r="X5" s="23">
         <f t="shared" ref="X5:Z10" si="7">100*(W5-$G5)/$G5</f>
-        <v>-100</v>
+        <v>7.9322201100469565</v>
       </c>
       <c r="Y5" s="21"/>
       <c r="Z5" s="23">
@@ -2287,10 +2305,12 @@
         <f t="shared" si="6"/>
         <v>13.882303699608672</v>
       </c>
-      <c r="W6" s="21"/>
+      <c r="W6" s="33">
+        <v>35.920999999999999</v>
+      </c>
       <c r="X6" s="23">
         <f t="shared" si="7"/>
-        <v>-100</v>
+        <v>10.097056496760768</v>
       </c>
       <c r="Y6" s="21"/>
       <c r="Z6" s="23">
@@ -2369,10 +2389,12 @@
         <f t="shared" si="6"/>
         <v>15.871011281031645</v>
       </c>
-      <c r="W7" s="21"/>
+      <c r="W7" s="33">
+        <v>8.4049999999999994</v>
+      </c>
       <c r="X7" s="23">
         <f t="shared" si="7"/>
-        <v>-99.999999999999986</v>
+        <v>8.9125307332890742</v>
       </c>
       <c r="Y7" s="21"/>
       <c r="Z7" s="23">
@@ -2451,10 +2473,12 @@
         <f t="shared" si="6"/>
         <v>21.617508208406662</v>
       </c>
-      <c r="W8" s="21"/>
+      <c r="W8" s="33">
+        <v>14.526999999999999</v>
+      </c>
       <c r="X8" s="23">
         <f t="shared" si="7"/>
-        <v>-100</v>
+        <v>12.602775127056951</v>
       </c>
       <c r="Y8" s="21"/>
       <c r="Z8" s="23">
@@ -2533,10 +2557,12 @@
         <f>100*(U9-$G9)/$G9</f>
         <v>44.749124509209487</v>
       </c>
-      <c r="W9" s="21"/>
+      <c r="W9" s="33">
+        <v>3.6309999999999998</v>
+      </c>
       <c r="X9" s="23">
         <f t="shared" si="7"/>
-        <v>-100</v>
+        <v>19.261191534590335</v>
       </c>
       <c r="Y9" s="21"/>
       <c r="Z9" s="23">
@@ -2615,10 +2641,12 @@
         <f t="shared" si="6"/>
         <v>12.543892964001783</v>
       </c>
-      <c r="W10" s="21"/>
+      <c r="W10" s="33">
+        <v>10.475</v>
+      </c>
       <c r="X10" s="23">
         <f t="shared" si="7"/>
-        <v>-100</v>
+        <v>4.2257341347289046</v>
       </c>
       <c r="Y10" s="21"/>
       <c r="Z10" s="23">
@@ -2687,7 +2715,7 @@
       </c>
       <c r="X12" s="3">
         <f t="shared" ref="X12" si="13">MIN(X4:X10)</f>
-        <v>-100</v>
+        <v>3.0736903751131559E-2</v>
       </c>
       <c r="Y12" s="2" t="s">
         <v>14</v>
@@ -2752,7 +2780,7 @@
       </c>
       <c r="X13" s="3">
         <f t="shared" ref="X13" si="20">AVERAGE(X4:X10)</f>
-        <v>-100</v>
+        <v>9.0088921486034454</v>
       </c>
       <c r="Y13" s="2" t="s">
         <v>15</v>
@@ -2817,7 +2845,7 @@
       </c>
       <c r="X14" s="3">
         <f t="shared" ref="X14" si="27">MAX(X4:X10)</f>
-        <v>-99.999999999999986</v>
+        <v>19.261191534590335</v>
       </c>
       <c r="Y14" s="2" t="s">
         <v>16</v>

</xml_diff>